<commit_message>
added trigger price for GTT orders
</commit_message>
<xml_diff>
--- a/GTT-ORDERS/GTT_ORDERS.xlsx
+++ b/GTT-ORDERS/GTT_ORDERS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anon\jupiter notebook files\practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anon\jupiter notebook files\practice\Swastika-API\GTT-ORDERS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28538D38-5824-468A-B59D-868E3BBBC366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D0283B-0AF1-4396-9FD4-56EED1F47F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{72E485CD-D213-43BE-83DF-5128678F1ACB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>SYMBOL</t>
   </si>
@@ -60,10 +60,10 @@
     <t>BUY</t>
   </si>
   <si>
-    <t>SELL</t>
-  </si>
-  <si>
     <t>NSE</t>
+  </si>
+  <si>
+    <t>TRIGGER_PRICE</t>
   </si>
 </sst>
 </file>
@@ -424,22 +424,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4CB264-C92C-433E-AEE4-12397A7D1899}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="3" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -450,16 +450,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -470,16 +473,19 @@
         <v>2</v>
       </c>
       <c r="D2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -490,16 +496,19 @@
         <v>3</v>
       </c>
       <c r="D3">
+        <v>3.1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -510,16 +519,19 @@
         <v>5</v>
       </c>
       <c r="D4">
+        <v>5.5</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -530,13 +542,16 @@
         <v>1</v>
       </c>
       <c r="D5">
+        <v>1.4</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
+      <c r="G5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>